<commit_message>
update and known BMS/BMN/BMN
</commit_message>
<xml_diff>
--- a/ongeki.xlsx
+++ b/ongeki.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540"/>
+    <workbookView windowWidth="28800" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="ongeki" sheetId="1" r:id="rId1"/>
@@ -433,7 +433,7 @@
     <t>BLT</t>
   </si>
   <si>
-    <t>(?)BeamStart</t>
+    <t>BeamStart 激光攻击起始标识</t>
   </si>
   <si>
     <t>recID 同id按组</t>
@@ -452,13 +452,13 @@
     <t>BMS</t>
   </si>
   <si>
-    <t>(?)BeamNext</t>
+    <t>BeamNext 激光攻击中继(移动)标识</t>
   </si>
   <si>
     <t>BMN</t>
   </si>
   <si>
-    <t>(?)BeamEnd</t>
+    <t>BeamEnd 激光攻击终止标识</t>
   </si>
   <si>
     <t>BME</t>
@@ -549,7 +549,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -559,27 +559,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -603,6 +582,35 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -633,16 +641,17 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -651,14 +660,6 @@
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -680,7 +681,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -693,29 +709,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -723,6 +716,66 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -732,7 +785,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -744,169 +887,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -935,24 +928,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -971,7 +946,36 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1006,168 +1010,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1176,9 +1169,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1519,1395 +1509,1395 @@
   <sheetPr/>
   <dimension ref="A1:N154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="F126" sqref="F126"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="B128" sqref="B128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="58.5" style="6" customWidth="1"/>
-    <col min="2" max="2" width="50.625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="34.5" style="6" customWidth="1"/>
-    <col min="4" max="4" width="21.125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.25" style="6" customWidth="1"/>
-    <col min="6" max="6" width="32.625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="18.25" style="6" customWidth="1"/>
-    <col min="8" max="8" width="20.375" style="6" customWidth="1"/>
-    <col min="9" max="9" width="15.5" style="6" customWidth="1"/>
-    <col min="10" max="10" width="13.375" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="6"/>
+    <col min="1" max="1" width="58.5" style="5" customWidth="1"/>
+    <col min="2" max="2" width="50.625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="34.5" style="5" customWidth="1"/>
+    <col min="4" max="4" width="21.125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="19.25" style="5" customWidth="1"/>
+    <col min="6" max="6" width="32.625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="18.25" style="5" customWidth="1"/>
+    <col min="8" max="8" width="20.375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="15.5" style="5" customWidth="1"/>
+    <col min="10" max="10" width="13.375" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" s="5" customFormat="1" spans="1:4">
-      <c r="A4" s="5" t="s">
+    <row r="4" s="4" customFormat="1" spans="1:4">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>3</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" s="5" customFormat="1" spans="1:2">
-      <c r="A7" s="5" t="s">
+    <row r="7" s="4" customFormat="1" spans="1:2">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" s="5" customFormat="1" spans="1:5">
-      <c r="A10" s="5" t="s">
+    <row r="10" s="4" customFormat="1" spans="1:5">
+      <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>180</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>180</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>180</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" s="5" customFormat="1" spans="1:3">
-      <c r="A13" s="5" t="s">
+    <row r="13" s="4" customFormat="1" spans="1:3">
+      <c r="A13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>4</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1" spans="1:2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" s="5" customFormat="1" spans="1:2">
-      <c r="A16" s="5" t="s">
+    <row r="16" s="4" customFormat="1" spans="1:2">
+      <c r="A16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>1920</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" s="5" customFormat="1" spans="1:2">
-      <c r="A19" s="5" t="s">
+    <row r="19" s="4" customFormat="1" spans="1:2">
+      <c r="A19" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <v>4096</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" s="5" customFormat="1" spans="1:2">
-      <c r="A22" s="5" t="s">
+    <row r="22" s="4" customFormat="1" spans="1:2">
+      <c r="A22" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="4">
         <v>1920</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" s="5" customFormat="1" spans="1:2">
-      <c r="A25" s="5" t="s">
+    <row r="25" s="4" customFormat="1" spans="1:2">
+      <c r="A25" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" s="5" customFormat="1" spans="1:2">
-      <c r="A28" s="5" t="s">
+    <row r="28" s="4" customFormat="1" spans="1:2">
+      <c r="A28" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="31" s="5" customFormat="1" spans="1:2">
-      <c r="A31" s="5" t="s">
+    <row r="31" s="4" customFormat="1" spans="1:2">
+      <c r="A31" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" s="5" customFormat="1" spans="1:2">
-      <c r="A34" s="5" t="s">
+    <row r="34" s="4" customFormat="1" spans="1:2">
+      <c r="A34" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" s="5" customFormat="1" spans="1:2">
-      <c r="A37" s="5" t="s">
+    <row r="37" s="4" customFormat="1" spans="1:2">
+      <c r="A37" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="40" s="5" customFormat="1" spans="1:2">
-      <c r="A40" s="5" t="s">
+    <row r="40" s="4" customFormat="1" spans="1:2">
+      <c r="A40" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="5">
+      <c r="B40" s="4">
         <v>240</v>
       </c>
     </row>
     <row r="42" ht="171" spans="1:7">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E42" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F42" s="7" t="s">
+      <c r="F42" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G42" s="7" t="s">
+      <c r="G42" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="43" s="5" customFormat="1" spans="1:7">
-      <c r="A43" s="5" t="s">
+    <row r="43" s="4" customFormat="1" spans="1:7">
+      <c r="A43" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D43" s="4">
         <v>0</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E43" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F43" s="5">
+      <c r="F43" s="4">
         <v>1</v>
       </c>
-      <c r="G43" s="5" t="s">
+      <c r="G43" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="46" s="5" customFormat="1" spans="1:1">
-      <c r="A46" s="5" t="s">
+    <row r="46" s="4" customFormat="1" spans="1:1">
+      <c r="A46" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D48" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" s="5" customFormat="1" spans="1:4">
-      <c r="A49" s="5" t="s">
+    <row r="49" s="4" customFormat="1" spans="1:4">
+      <c r="A49" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B49" s="5">
+      <c r="B49" s="4">
         <v>85</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C49" s="4">
         <v>0</v>
       </c>
-      <c r="D49" s="5">
+      <c r="D49" s="4">
         <v>240</v>
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="6" t="s">
+      <c r="A51" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C51" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D51" s="6" t="s">
+      <c r="D51" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E51" s="6" t="s">
+      <c r="E51" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="52" s="5" customFormat="1" spans="1:5">
-      <c r="A52" s="5" t="s">
+    <row r="52" s="4" customFormat="1" spans="1:5">
+      <c r="A52" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B52" s="4">
         <v>0</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C52" s="4">
         <v>0</v>
       </c>
-      <c r="D52" s="5">
+      <c r="D52" s="4">
         <v>4</v>
       </c>
-      <c r="E52" s="5">
+      <c r="E52" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="6" t="s">
+      <c r="A54" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="55" s="5" customFormat="1" spans="1:3">
-      <c r="A55" s="5" t="s">
+    <row r="55" s="4" customFormat="1" spans="1:3">
+      <c r="A55" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="5">
+      <c r="B55" s="4">
         <v>0</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C55" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="6" t="s">
+      <c r="A57" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C57" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="D57" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E57" s="6" t="s">
+      <c r="E57" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="58" s="5" customFormat="1" spans="1:5">
-      <c r="A58" s="5" t="s">
+    <row r="58" s="4" customFormat="1" spans="1:5">
+      <c r="A58" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B58" s="5">
+      <c r="B58" s="4">
         <v>0</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C58" s="4">
         <v>0</v>
       </c>
-      <c r="D58" s="5">
+      <c r="D58" s="4">
         <v>240</v>
       </c>
-      <c r="E58" s="5">
+      <c r="E58" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="60" ht="85.5" customHeight="1" spans="1:4">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B60" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C60" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="61" s="5" customFormat="1" spans="1:4">
-      <c r="A61" s="5" t="s">
+    <row r="61" s="4" customFormat="1" spans="1:4">
+      <c r="A61" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B61" s="5">
+      <c r="B61" s="4">
         <v>0</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C61" s="4">
         <v>0</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D61" s="4" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="63" spans="1:14">
-      <c r="A63" s="6" t="s">
+      <c r="A63" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C63" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D63" s="6" t="s">
+      <c r="D63" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E63" s="6" t="s">
+      <c r="E63" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="G63" s="8"/>
-      <c r="H63" s="8"/>
-      <c r="I63" s="8"/>
-      <c r="J63" s="8"/>
-      <c r="K63" s="8"/>
-      <c r="L63" s="8"/>
-      <c r="M63" s="8"/>
-      <c r="N63" s="8"/>
-    </row>
-    <row r="64" s="5" customFormat="1" spans="1:14">
-      <c r="A64" s="5" t="s">
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
+      <c r="I63" s="7"/>
+      <c r="J63" s="7"/>
+      <c r="K63" s="7"/>
+      <c r="L63" s="7"/>
+      <c r="M63" s="7"/>
+      <c r="N63" s="7"/>
+    </row>
+    <row r="64" s="4" customFormat="1" spans="1:14">
+      <c r="A64" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B64" s="5">
+      <c r="B64" s="4">
         <v>173</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C64" s="4">
         <v>1</v>
       </c>
-      <c r="D64" s="5">
+      <c r="D64" s="4">
         <v>960</v>
       </c>
-      <c r="E64" s="5">
+      <c r="E64" s="4">
         <v>-24</v>
       </c>
-      <c r="G64" s="8"/>
-      <c r="H64" s="8"/>
-      <c r="I64" s="8"/>
-      <c r="J64" s="8"/>
-      <c r="K64" s="8"/>
-      <c r="L64" s="8"/>
-      <c r="M64" s="8"/>
-      <c r="N64" s="8"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+      <c r="I64" s="7"/>
+      <c r="J64" s="7"/>
+      <c r="K64" s="7"/>
+      <c r="L64" s="7"/>
+      <c r="M64" s="7"/>
+      <c r="N64" s="7"/>
     </row>
     <row r="65" spans="7:14">
-      <c r="G65" s="8"/>
-      <c r="H65" s="8"/>
-      <c r="I65" s="8"/>
-      <c r="J65" s="8"/>
-      <c r="K65" s="8"/>
-      <c r="L65" s="8"/>
-      <c r="M65" s="8"/>
-      <c r="N65" s="8"/>
+      <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
+      <c r="I65" s="7"/>
+      <c r="J65" s="7"/>
+      <c r="K65" s="7"/>
+      <c r="L65" s="7"/>
+      <c r="M65" s="7"/>
+      <c r="N65" s="7"/>
     </row>
     <row r="66" spans="1:14">
-      <c r="A66" s="6" t="s">
+      <c r="A66" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="B66" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C66" s="9"/>
-      <c r="D66" s="9"/>
-      <c r="E66" s="9"/>
-      <c r="G66" s="8"/>
-      <c r="H66" s="8"/>
-      <c r="I66" s="8"/>
-      <c r="J66" s="8"/>
-      <c r="K66" s="8"/>
-      <c r="L66" s="8"/>
-      <c r="M66" s="8"/>
-      <c r="N66" s="8"/>
-    </row>
-    <row r="67" s="5" customFormat="1" spans="1:14">
-      <c r="A67" s="5" t="s">
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+      <c r="G66" s="7"/>
+      <c r="H66" s="7"/>
+      <c r="I66" s="7"/>
+      <c r="J66" s="7"/>
+      <c r="K66" s="7"/>
+      <c r="L66" s="7"/>
+      <c r="M66" s="7"/>
+      <c r="N66" s="7"/>
+    </row>
+    <row r="67" s="4" customFormat="1" spans="1:14">
+      <c r="A67" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B67" s="9"/>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-      <c r="G67" s="8"/>
-      <c r="H67" s="8"/>
-      <c r="I67" s="8"/>
-      <c r="J67" s="8"/>
-      <c r="K67" s="8"/>
-      <c r="L67" s="8"/>
-      <c r="M67" s="8"/>
-      <c r="N67" s="8"/>
+      <c r="B67" s="8"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="7"/>
+      <c r="I67" s="7"/>
+      <c r="J67" s="7"/>
+      <c r="K67" s="7"/>
+      <c r="L67" s="7"/>
+      <c r="M67" s="7"/>
+      <c r="N67" s="7"/>
     </row>
     <row r="68" spans="7:14">
-      <c r="G68" s="8"/>
-      <c r="H68" s="8"/>
-      <c r="I68" s="8"/>
-      <c r="J68" s="8"/>
-      <c r="K68" s="8"/>
-      <c r="L68" s="8"/>
-      <c r="M68" s="8"/>
-      <c r="N68" s="8"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
+      <c r="I68" s="7"/>
+      <c r="J68" s="7"/>
+      <c r="K68" s="7"/>
+      <c r="L68" s="7"/>
+      <c r="M68" s="7"/>
+      <c r="N68" s="7"/>
     </row>
     <row r="69" spans="1:14">
-      <c r="A69" s="6" t="s">
+      <c r="A69" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B69" s="9" t="s">
+      <c r="B69" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C69" s="9"/>
-      <c r="D69" s="9"/>
-      <c r="E69" s="9"/>
-      <c r="G69" s="8"/>
-      <c r="H69" s="8"/>
-      <c r="I69" s="8"/>
-      <c r="J69" s="8"/>
-      <c r="K69" s="8"/>
-      <c r="L69" s="8"/>
-      <c r="M69" s="8"/>
-      <c r="N69" s="8"/>
-    </row>
-    <row r="70" s="5" customFormat="1" spans="1:14">
-      <c r="A70" s="5" t="s">
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8"/>
+      <c r="G69" s="7"/>
+      <c r="H69" s="7"/>
+      <c r="I69" s="7"/>
+      <c r="J69" s="7"/>
+      <c r="K69" s="7"/>
+      <c r="L69" s="7"/>
+      <c r="M69" s="7"/>
+      <c r="N69" s="7"/>
+    </row>
+    <row r="70" s="4" customFormat="1" spans="1:14">
+      <c r="A70" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B70" s="9"/>
-      <c r="C70" s="9"/>
-      <c r="D70" s="9"/>
-      <c r="E70" s="9"/>
-      <c r="G70" s="8"/>
-      <c r="H70" s="8"/>
-      <c r="I70" s="8"/>
-      <c r="J70" s="8"/>
-      <c r="K70" s="8"/>
-      <c r="L70" s="8"/>
-      <c r="M70" s="8"/>
-      <c r="N70" s="8"/>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+      <c r="G70" s="7"/>
+      <c r="H70" s="7"/>
+      <c r="I70" s="7"/>
+      <c r="J70" s="7"/>
+      <c r="K70" s="7"/>
+      <c r="L70" s="7"/>
+      <c r="M70" s="7"/>
+      <c r="N70" s="7"/>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="6" t="s">
+      <c r="A72" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B72" s="9" t="s">
+      <c r="B72" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C72" s="9"/>
-      <c r="D72" s="9"/>
-      <c r="E72" s="9"/>
-    </row>
-    <row r="73" s="5" customFormat="1" spans="1:5">
-      <c r="A73" s="5" t="s">
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+    </row>
+    <row r="73" s="4" customFormat="1" spans="1:5">
+      <c r="A73" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B73" s="9"/>
-      <c r="C73" s="9"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="9"/>
+      <c r="B73" s="8"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="8"/>
     </row>
     <row r="75" spans="1:5">
-      <c r="A75" s="6" t="s">
+      <c r="A75" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B75" s="9" t="s">
+      <c r="B75" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C75" s="9"/>
-      <c r="D75" s="9"/>
-      <c r="E75" s="9"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8"/>
+      <c r="E75" s="8"/>
     </row>
     <row r="76" spans="1:5">
-      <c r="A76" s="5" t="s">
+      <c r="A76" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B76" s="9"/>
-      <c r="C76" s="9"/>
-      <c r="D76" s="9"/>
-      <c r="E76" s="9"/>
+      <c r="B76" s="8"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="8"/>
     </row>
     <row r="78" spans="1:5">
-      <c r="A78" s="6" t="s">
+      <c r="A78" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B78" s="9" t="s">
+      <c r="B78" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C78" s="9"/>
-      <c r="D78" s="9"/>
-      <c r="E78" s="9"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
     </row>
     <row r="79" spans="1:5">
-      <c r="A79" s="5" t="s">
+      <c r="A79" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B79" s="9"/>
-      <c r="C79" s="9"/>
-      <c r="D79" s="9"/>
-      <c r="E79" s="9"/>
+      <c r="B79" s="8"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="8"/>
     </row>
     <row r="81" spans="1:5">
-      <c r="A81" s="6" t="s">
+      <c r="A81" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B81" s="9" t="s">
+      <c r="B81" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C81" s="9"/>
-      <c r="D81" s="9"/>
-      <c r="E81" s="9"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="8"/>
+      <c r="E81" s="8"/>
     </row>
     <row r="82" spans="1:5">
-      <c r="A82" s="5" t="s">
+      <c r="A82" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B82" s="9"/>
-      <c r="C82" s="9"/>
-      <c r="D82" s="9"/>
-      <c r="E82" s="9"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8"/>
     </row>
     <row r="84" spans="1:5">
-      <c r="A84" s="6" t="s">
+      <c r="A84" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B84" s="9" t="s">
+      <c r="B84" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C84" s="9"/>
-      <c r="D84" s="9"/>
-      <c r="E84" s="9"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
+      <c r="E84" s="8"/>
     </row>
     <row r="85" spans="1:5">
-      <c r="A85" s="5" t="s">
+      <c r="A85" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B85" s="9"/>
-      <c r="C85" s="9"/>
-      <c r="D85" s="9"/>
-      <c r="E85" s="9"/>
+      <c r="B85" s="8"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="8"/>
+      <c r="E85" s="8"/>
     </row>
     <row r="87" spans="1:5">
-      <c r="A87" s="6" t="s">
+      <c r="A87" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B87" s="9" t="s">
+      <c r="B87" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C87" s="9"/>
-      <c r="D87" s="9"/>
-      <c r="E87" s="9"/>
+      <c r="C87" s="8"/>
+      <c r="D87" s="8"/>
+      <c r="E87" s="8"/>
     </row>
     <row r="88" spans="1:5">
-      <c r="A88" s="5" t="s">
+      <c r="A88" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B88" s="9"/>
-      <c r="C88" s="9"/>
-      <c r="D88" s="9"/>
-      <c r="E88" s="9"/>
+      <c r="B88" s="8"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="8"/>
     </row>
     <row r="90" spans="1:5">
-      <c r="A90" s="6" t="s">
+      <c r="A90" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B90" s="9" t="s">
+      <c r="B90" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C90" s="9"/>
-      <c r="D90" s="9"/>
-      <c r="E90" s="9"/>
-    </row>
-    <row r="91" s="5" customFormat="1" spans="1:5">
-      <c r="A91" s="5" t="s">
+      <c r="C90" s="8"/>
+      <c r="D90" s="8"/>
+      <c r="E90" s="8"/>
+    </row>
+    <row r="91" s="4" customFormat="1" spans="1:5">
+      <c r="A91" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B91" s="9"/>
-      <c r="C91" s="9"/>
-      <c r="D91" s="9"/>
-      <c r="E91" s="9"/>
+      <c r="B91" s="8"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="8"/>
+      <c r="E91" s="8"/>
     </row>
     <row r="93" spans="1:5">
-      <c r="A93" s="6" t="s">
+      <c r="A93" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B93" s="9" t="s">
+      <c r="B93" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C93" s="9"/>
-      <c r="D93" s="9"/>
-      <c r="E93" s="9"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="8"/>
+      <c r="E93" s="8"/>
     </row>
     <row r="94" spans="1:5">
-      <c r="A94" s="5" t="s">
+      <c r="A94" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B94" s="9"/>
-      <c r="C94" s="9"/>
-      <c r="D94" s="9"/>
-      <c r="E94" s="9"/>
+      <c r="B94" s="8"/>
+      <c r="C94" s="8"/>
+      <c r="D94" s="8"/>
+      <c r="E94" s="8"/>
     </row>
     <row r="96" spans="1:5">
-      <c r="A96" s="6" t="s">
+      <c r="A96" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B96" s="9" t="s">
+      <c r="B96" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C96" s="9"/>
-      <c r="D96" s="9"/>
-      <c r="E96" s="9"/>
+      <c r="C96" s="8"/>
+      <c r="D96" s="8"/>
+      <c r="E96" s="8"/>
     </row>
     <row r="97" spans="1:5">
-      <c r="A97" s="5" t="s">
+      <c r="A97" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B97" s="9"/>
-      <c r="C97" s="9"/>
-      <c r="D97" s="9"/>
-      <c r="E97" s="9"/>
+      <c r="B97" s="8"/>
+      <c r="C97" s="8"/>
+      <c r="D97" s="8"/>
+      <c r="E97" s="8"/>
     </row>
     <row r="99" spans="1:5">
-      <c r="A99" s="6" t="s">
+      <c r="A99" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B99" s="9" t="s">
+      <c r="B99" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C99" s="9"/>
-      <c r="D99" s="9"/>
-      <c r="E99" s="9"/>
-    </row>
-    <row r="100" s="5" customFormat="1" spans="1:5">
-      <c r="A100" s="5" t="s">
+      <c r="C99" s="8"/>
+      <c r="D99" s="8"/>
+      <c r="E99" s="8"/>
+    </row>
+    <row r="100" s="4" customFormat="1" spans="1:5">
+      <c r="A100" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B100" s="9"/>
-      <c r="C100" s="9"/>
-      <c r="D100" s="9"/>
-      <c r="E100" s="9"/>
+      <c r="B100" s="8"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="8"/>
     </row>
     <row r="102" spans="1:5">
-      <c r="A102" s="6" t="s">
+      <c r="A102" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B102" s="9" t="s">
+      <c r="B102" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C102" s="9"/>
-      <c r="D102" s="9"/>
-      <c r="E102" s="9"/>
+      <c r="C102" s="8"/>
+      <c r="D102" s="8"/>
+      <c r="E102" s="8"/>
     </row>
     <row r="103" spans="1:5">
-      <c r="A103" s="5" t="s">
+      <c r="A103" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B103" s="9"/>
-      <c r="C103" s="9"/>
-      <c r="D103" s="9"/>
-      <c r="E103" s="9"/>
+      <c r="B103" s="8"/>
+      <c r="C103" s="8"/>
+      <c r="D103" s="8"/>
+      <c r="E103" s="8"/>
     </row>
     <row r="105" spans="1:5">
-      <c r="A105" s="6" t="s">
+      <c r="A105" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B105" s="9" t="s">
+      <c r="B105" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C105" s="9"/>
-      <c r="D105" s="9"/>
-      <c r="E105" s="9"/>
+      <c r="C105" s="8"/>
+      <c r="D105" s="8"/>
+      <c r="E105" s="8"/>
     </row>
     <row r="106" spans="1:5">
-      <c r="A106" s="5" t="s">
+      <c r="A106" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B106" s="9"/>
-      <c r="C106" s="9"/>
-      <c r="D106" s="9"/>
-      <c r="E106" s="9"/>
+      <c r="B106" s="8"/>
+      <c r="C106" s="8"/>
+      <c r="D106" s="8"/>
+      <c r="E106" s="8"/>
     </row>
     <row r="108" spans="1:5">
-      <c r="A108" s="6" t="s">
+      <c r="A108" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B108" s="9" t="s">
+      <c r="B108" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C108" s="9"/>
-      <c r="D108" s="9"/>
-      <c r="E108" s="9"/>
-    </row>
-    <row r="109" s="5" customFormat="1" spans="1:5">
-      <c r="A109" s="5" t="s">
+      <c r="C108" s="8"/>
+      <c r="D108" s="8"/>
+      <c r="E108" s="8"/>
+    </row>
+    <row r="109" s="4" customFormat="1" spans="1:5">
+      <c r="A109" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B109" s="9"/>
-      <c r="C109" s="9"/>
-      <c r="D109" s="9"/>
-      <c r="E109" s="9"/>
+      <c r="B109" s="8"/>
+      <c r="C109" s="8"/>
+      <c r="D109" s="8"/>
+      <c r="E109" s="8"/>
     </row>
     <row r="111" spans="1:5">
-      <c r="A111" s="6" t="s">
+      <c r="A111" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B111" s="9" t="s">
+      <c r="B111" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C111" s="9"/>
-      <c r="D111" s="9"/>
-      <c r="E111" s="9"/>
-    </row>
-    <row r="112" s="5" customFormat="1" spans="1:5">
-      <c r="A112" s="5" t="s">
+      <c r="C111" s="8"/>
+      <c r="D111" s="8"/>
+      <c r="E111" s="8"/>
+    </row>
+    <row r="112" s="4" customFormat="1" spans="1:5">
+      <c r="A112" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B112" s="9"/>
-      <c r="C112" s="9"/>
-      <c r="D112" s="9"/>
-      <c r="E112" s="9"/>
+      <c r="B112" s="8"/>
+      <c r="C112" s="8"/>
+      <c r="D112" s="8"/>
+      <c r="E112" s="8"/>
     </row>
     <row r="114" spans="1:5">
-      <c r="A114" s="6" t="s">
+      <c r="A114" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B114" s="9" t="s">
+      <c r="B114" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C114" s="9"/>
-      <c r="D114" s="9"/>
-      <c r="E114" s="9"/>
-    </row>
-    <row r="115" s="5" customFormat="1" spans="1:5">
-      <c r="A115" s="5" t="s">
+      <c r="C114" s="8"/>
+      <c r="D114" s="8"/>
+      <c r="E114" s="8"/>
+    </row>
+    <row r="115" s="4" customFormat="1" spans="1:5">
+      <c r="A115" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B115" s="9"/>
-      <c r="C115" s="9"/>
-      <c r="D115" s="9"/>
-      <c r="E115" s="9"/>
+      <c r="B115" s="8"/>
+      <c r="C115" s="8"/>
+      <c r="D115" s="8"/>
+      <c r="E115" s="8"/>
     </row>
     <row r="117" spans="1:10">
-      <c r="A117" s="6" t="s">
+      <c r="A117" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B117" s="6" t="s">
+      <c r="B117" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C117" s="6" t="s">
+      <c r="C117" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D117" s="6" t="s">
+      <c r="D117" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E117" s="6" t="s">
+      <c r="E117" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="F117" s="6" t="s">
+      <c r="F117" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="G117" s="6" t="s">
+      <c r="G117" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="H117" s="6" t="s">
+      <c r="H117" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="I117" s="6" t="s">
+      <c r="I117" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="J117" s="6" t="s">
+      <c r="J117" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="118" s="5" customFormat="1" spans="1:10">
-      <c r="A118" s="5" t="s">
+    <row r="118" s="4" customFormat="1" spans="1:10">
+      <c r="A118" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B118" s="5">
+      <c r="B118" s="4">
         <v>173</v>
       </c>
-      <c r="C118" s="5">
+      <c r="C118" s="4">
         <v>92</v>
       </c>
-      <c r="D118" s="5">
+      <c r="D118" s="4">
         <v>1440</v>
       </c>
-      <c r="E118" s="5">
+      <c r="E118" s="4">
         <v>24</v>
       </c>
-      <c r="F118" s="5">
+      <c r="F118" s="4">
         <v>0</v>
       </c>
-      <c r="G118" s="5">
+      <c r="G118" s="4">
         <v>93</v>
       </c>
-      <c r="H118" s="5">
+      <c r="H118" s="4">
         <v>0</v>
       </c>
-      <c r="I118" s="5">
+      <c r="I118" s="4">
         <v>24</v>
       </c>
-      <c r="J118" s="5">
+      <c r="J118" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:10">
-      <c r="A120" s="6" t="s">
+      <c r="A120" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B120" s="9" t="s">
+      <c r="B120" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C120" s="9"/>
-      <c r="D120" s="9"/>
-      <c r="E120" s="9"/>
-      <c r="F120" s="9"/>
-      <c r="G120" s="9"/>
-      <c r="H120" s="9"/>
-      <c r="I120" s="9"/>
-      <c r="J120" s="9"/>
+      <c r="C120" s="8"/>
+      <c r="D120" s="8"/>
+      <c r="E120" s="8"/>
+      <c r="F120" s="8"/>
+      <c r="G120" s="8"/>
+      <c r="H120" s="8"/>
+      <c r="I120" s="8"/>
+      <c r="J120" s="8"/>
     </row>
     <row r="121" spans="1:10">
-      <c r="A121" s="5" t="s">
+      <c r="A121" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B121" s="9"/>
-      <c r="C121" s="9"/>
-      <c r="D121" s="9"/>
-      <c r="E121" s="9"/>
-      <c r="F121" s="9"/>
-      <c r="G121" s="9"/>
-      <c r="H121" s="9"/>
-      <c r="I121" s="9"/>
-      <c r="J121" s="9"/>
+      <c r="B121" s="8"/>
+      <c r="C121" s="8"/>
+      <c r="D121" s="8"/>
+      <c r="E121" s="8"/>
+      <c r="F121" s="8"/>
+      <c r="G121" s="8"/>
+      <c r="H121" s="8"/>
+      <c r="I121" s="8"/>
+      <c r="J121" s="8"/>
     </row>
     <row r="123" spans="1:5">
-      <c r="A123" s="6" t="s">
+      <c r="A123" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B123" s="6" t="s">
+      <c r="B123" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="C123" s="6" t="s">
+      <c r="C123" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D123" s="6" t="s">
+      <c r="D123" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E123" s="6" t="s">
+      <c r="E123" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="124" s="5" customFormat="1" spans="1:5">
-      <c r="A124" s="5" t="s">
+    <row r="124" s="4" customFormat="1" spans="1:5">
+      <c r="A124" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B124" s="5" t="s">
+      <c r="B124" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C124" s="5">
+      <c r="C124" s="4">
         <v>30</v>
       </c>
-      <c r="D124" s="5">
+      <c r="D124" s="4">
         <v>960</v>
       </c>
-      <c r="E124" s="5">
+      <c r="E124" s="4">
         <v>-24</v>
       </c>
     </row>
     <row r="126" ht="156.75" spans="1:6">
-      <c r="A126" s="6" t="s">
+      <c r="A126" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B126" s="6" t="s">
+      <c r="B126" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C126" s="6" t="s">
+      <c r="C126" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D126" s="6" t="s">
+      <c r="D126" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E126" s="6" t="s">
+      <c r="E126" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F126" s="7" t="s">
+      <c r="F126" s="6" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="127" s="5" customFormat="1" spans="1:6">
-      <c r="A127" s="5" t="s">
+    <row r="127" s="4" customFormat="1" spans="1:6">
+      <c r="A127" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B127" s="5">
+      <c r="B127" s="4">
         <v>0</v>
       </c>
-      <c r="C127" s="5">
+      <c r="C127" s="4">
         <v>117</v>
       </c>
-      <c r="D127" s="5">
+      <c r="D127" s="4">
         <v>960</v>
       </c>
-      <c r="E127" s="5">
+      <c r="E127" s="4">
         <v>-40</v>
       </c>
-      <c r="F127" s="5">
+      <c r="F127" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="129" spans="1:5">
-      <c r="A129" s="6" t="s">
+      <c r="A129" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B129" s="6" t="s">
+      <c r="B129" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C129" s="6" t="s">
+      <c r="C129" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D129" s="6" t="s">
+      <c r="D129" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E129" s="6" t="s">
+      <c r="E129" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="130" s="5" customFormat="1" spans="1:5">
-      <c r="A130" s="5" t="s">
+    <row r="130" s="4" customFormat="1" spans="1:5">
+      <c r="A130" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B130" s="5">
+      <c r="B130" s="4">
         <v>0</v>
       </c>
-      <c r="C130" s="5">
+      <c r="C130" s="4">
         <v>117</v>
       </c>
-      <c r="D130" s="5">
+      <c r="D130" s="4">
         <v>960</v>
       </c>
-      <c r="E130" s="5">
+      <c r="E130" s="4">
         <v>-40</v>
       </c>
     </row>
     <row r="132" spans="1:5">
-      <c r="A132" s="6" t="s">
+      <c r="A132" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B132" s="6" t="s">
+      <c r="B132" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C132" s="6" t="s">
+      <c r="C132" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D132" s="6" t="s">
+      <c r="D132" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E132" s="6" t="s">
+      <c r="E132" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="133" s="5" customFormat="1" spans="1:5">
-      <c r="A133" s="5" t="s">
+    <row r="133" s="4" customFormat="1" spans="1:5">
+      <c r="A133" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B133" s="5">
+      <c r="B133" s="4">
         <v>0</v>
       </c>
-      <c r="C133" s="5">
+      <c r="C133" s="4">
         <v>117</v>
       </c>
-      <c r="D133" s="5">
+      <c r="D133" s="4">
         <v>960</v>
       </c>
-      <c r="E133" s="5">
+      <c r="E133" s="4">
         <v>-40</v>
       </c>
     </row>
     <row r="135" spans="1:4">
-      <c r="A135" s="6" t="s">
+      <c r="A135" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B135" s="6" t="s">
+      <c r="B135" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C135" s="6" t="s">
+      <c r="C135" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D135" s="6" t="s">
+      <c r="D135" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="136" s="5" customFormat="1" spans="1:4">
-      <c r="A136" s="5" t="s">
+    <row r="136" s="4" customFormat="1" spans="1:4">
+      <c r="A136" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B136" s="5">
+      <c r="B136" s="4">
         <v>3</v>
       </c>
-      <c r="C136" s="5">
+      <c r="C136" s="4">
         <v>1440</v>
       </c>
-      <c r="D136" s="5">
+      <c r="D136" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="138" ht="42.75" spans="1:5">
-      <c r="A138" s="7" t="s">
+      <c r="A138" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="B138" s="6" t="s">
+      <c r="B138" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C138" s="6" t="s">
+      <c r="C138" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D138" s="6" t="s">
+      <c r="D138" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E138" s="7" t="s">
+      <c r="E138" s="6" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="139" s="5" customFormat="1" spans="1:5">
-      <c r="A139" s="5" t="s">
+    <row r="139" s="4" customFormat="1" spans="1:5">
+      <c r="A139" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B139" s="5">
+      <c r="B139" s="4">
         <v>26</v>
       </c>
-      <c r="C139" s="5">
+      <c r="C139" s="4">
         <v>960</v>
       </c>
-      <c r="D139" s="5">
+      <c r="D139" s="4">
         <v>-8</v>
       </c>
-      <c r="E139" s="5" t="s">
+      <c r="E139" s="4" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="141" spans="1:5">
-      <c r="A141" s="6" t="s">
+      <c r="A141" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="B141" s="9" t="s">
+      <c r="B141" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C141" s="9"/>
-      <c r="D141" s="9"/>
-      <c r="E141" s="9"/>
-    </row>
-    <row r="142" s="5" customFormat="1" spans="1:5">
-      <c r="A142" s="5" t="s">
+      <c r="C141" s="8"/>
+      <c r="D141" s="8"/>
+      <c r="E141" s="8"/>
+    </row>
+    <row r="142" s="4" customFormat="1" spans="1:5">
+      <c r="A142" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B142" s="9"/>
-      <c r="C142" s="9"/>
-      <c r="D142" s="9"/>
-      <c r="E142" s="9"/>
+      <c r="B142" s="8"/>
+      <c r="C142" s="8"/>
+      <c r="D142" s="8"/>
+      <c r="E142" s="8"/>
     </row>
     <row r="143" spans="1:4">
-      <c r="A143" s="5"/>
-      <c r="D143" s="8"/>
+      <c r="A143" s="4"/>
+      <c r="D143" s="7"/>
     </row>
     <row r="144" spans="1:6">
-      <c r="A144" s="6" t="s">
+      <c r="A144" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B144" s="6" t="s">
+      <c r="B144" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="C144" s="6" t="s">
+      <c r="C144" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D144" s="6" t="s">
+      <c r="D144" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E144" s="6" t="s">
+      <c r="E144" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F144" s="6" t="s">
+      <c r="F144" s="5" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="145" spans="1:6">
-      <c r="A145" s="6" t="s">
+      <c r="A145" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="B145" s="6">
+      <c r="B145" s="5">
         <v>72</v>
       </c>
-      <c r="C145" s="6">
+      <c r="C145" s="5">
         <v>11</v>
       </c>
-      <c r="D145" s="6">
+      <c r="D145" s="5">
         <v>1440</v>
       </c>
-      <c r="E145" s="6">
+      <c r="E145" s="5">
         <v>24</v>
       </c>
-      <c r="F145" s="6">
+      <c r="F145" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:6">
-      <c r="A147" s="6" t="s">
+      <c r="A147" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="B147" s="9" t="s">
+      <c r="B147" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C147" s="9"/>
-      <c r="D147" s="9"/>
-      <c r="E147" s="9"/>
-      <c r="F147" s="9"/>
+      <c r="C147" s="8"/>
+      <c r="D147" s="8"/>
+      <c r="E147" s="8"/>
+      <c r="F147" s="8"/>
     </row>
     <row r="148" spans="1:6">
-      <c r="A148" s="6" t="s">
+      <c r="A148" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="B148" s="9"/>
-      <c r="C148" s="9"/>
-      <c r="D148" s="9"/>
-      <c r="E148" s="9"/>
-      <c r="F148" s="9"/>
+      <c r="B148" s="8"/>
+      <c r="C148" s="8"/>
+      <c r="D148" s="8"/>
+      <c r="E148" s="8"/>
+      <c r="F148" s="8"/>
     </row>
     <row r="150" spans="1:10">
-      <c r="A150" s="6" t="s">
+      <c r="A150" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B150" s="6" t="s">
+      <c r="B150" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="C150" s="6" t="s">
+      <c r="C150" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D150" s="6" t="s">
+      <c r="D150" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E150" s="6" t="s">
+      <c r="E150" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="F150" s="6" t="s">
+      <c r="F150" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="G150" s="6" t="s">
+      <c r="G150" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="H150" s="6" t="s">
+      <c r="H150" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="I150" s="6" t="s">
+      <c r="I150" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="J150" s="6" t="s">
+      <c r="J150" s="5" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="151" spans="1:10">
-      <c r="A151" s="6" t="s">
+      <c r="A151" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B151" s="6">
+      <c r="B151" s="5">
         <v>151</v>
       </c>
-      <c r="C151" s="6">
+      <c r="C151" s="5">
         <v>1</v>
       </c>
-      <c r="D151" s="6">
+      <c r="D151" s="5">
         <v>1200</v>
       </c>
-      <c r="E151" s="6">
+      <c r="E151" s="5">
         <v>-12</v>
       </c>
-      <c r="F151" s="6">
+      <c r="F151" s="5">
         <v>0</v>
       </c>
-      <c r="G151" s="6">
+      <c r="G151" s="5">
         <v>1</v>
       </c>
-      <c r="H151" s="6">
+      <c r="H151" s="5">
         <v>1680</v>
       </c>
-      <c r="I151" s="6">
+      <c r="I151" s="5">
         <v>-12</v>
       </c>
-      <c r="J151" s="6">
+      <c r="J151" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:10">
-      <c r="A153" s="6" t="s">
+      <c r="A153" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="B153" s="9" t="s">
+      <c r="B153" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C153" s="9"/>
-      <c r="D153" s="9"/>
-      <c r="E153" s="9"/>
-      <c r="F153" s="9"/>
-      <c r="G153" s="9"/>
-      <c r="H153" s="9"/>
-      <c r="I153" s="9"/>
-      <c r="J153" s="9"/>
+      <c r="C153" s="8"/>
+      <c r="D153" s="8"/>
+      <c r="E153" s="8"/>
+      <c r="F153" s="8"/>
+      <c r="G153" s="8"/>
+      <c r="H153" s="8"/>
+      <c r="I153" s="8"/>
+      <c r="J153" s="8"/>
     </row>
     <row r="154" spans="1:10">
-      <c r="A154" s="6" t="s">
+      <c r="A154" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="B154" s="9"/>
-      <c r="C154" s="9"/>
-      <c r="D154" s="9"/>
-      <c r="E154" s="9"/>
-      <c r="F154" s="9"/>
-      <c r="G154" s="9"/>
-      <c r="H154" s="9"/>
-      <c r="I154" s="9"/>
-      <c r="J154" s="9"/>
+      <c r="B154" s="8"/>
+      <c r="C154" s="8"/>
+      <c r="D154" s="8"/>
+      <c r="E154" s="8"/>
+      <c r="F154" s="8"/>
+      <c r="G154" s="8"/>
+      <c r="H154" s="8"/>
+      <c r="I154" s="8"/>
+      <c r="J154" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -2975,7 +2965,6 @@
       <c r="N1" t="s">
         <v>160</v>
       </c>
-      <c r="O1"/>
       <c r="P1" t="s">
         <v>60</v>
       </c>
@@ -3000,7 +2989,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
-      <c r="N2" s="4">
+      <c r="N2" s="3">
         <f>O2*P2/(Q2*R2)</f>
         <v>1875</v>
       </c>

</xml_diff>